<commit_message>
Bugfixed tests, updated TestBook1
</commit_message>
<xml_diff>
--- a/test_resources/TestBook1.xlsx
+++ b/test_resources/TestBook1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>2a</t>
   </si>
@@ -56,10 +56,17 @@
     <t>c3</t>
   </si>
   <si>
-    <t>c4</t>
-  </si>
-  <si>
     <t>c5</t>
+  </si>
+  <si>
+    <t>b5</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+whitespace    string</t>
   </si>
 </sst>
 </file>
@@ -95,9 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,6 +201,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -226,6 +253,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -378,20 +422,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -405,7 +452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -415,8 +462,14 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
+      <c r="D3">
+        <v>123456</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -424,15 +477,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Cell.value_without_whitespace, added whitespace tests for Cell.
</commit_message>
<xml_diff>
--- a/test_resources/TestBook1.xlsx
+++ b/test_resources/TestBook1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>2a</t>
   </si>
@@ -67,6 +67,9 @@
   <si>
     <t xml:space="preserve">
 whitespace    string</t>
+  </si>
+  <si>
+    <t>whitespace    string</t>
   </si>
 </sst>
 </file>
@@ -422,23 +425,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -452,7 +456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -468,8 +472,11 @@
       <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -477,7 +484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>

</xml_diff>